<commit_message>
Update project06 - 프로젝트 진행 현황.xlsx
</commit_message>
<xml_diff>
--- a/4. 진행현황/project06 - 프로젝트 진행 현황.xlsx
+++ b/4. 진행현황/project06 - 프로젝트 진행 현황.xlsx
@@ -959,10 +959,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>형준  + 현태</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>2. 구현 현황</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -974,6 +970,10 @@
     <t>화면 설계</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>형준  +  현태</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -982,7 +982,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1125,17 +1125,9 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="돋움"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Dotum"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
@@ -2258,6 +2250,21 @@
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2288,26 +2295,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2317,39 +2312,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2387,65 +2349,50 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2455,6 +2402,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2466,6 +2419,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2487,6 +2455,69 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2515,30 +2546,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2570,46 +2577,31 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2835,8 +2827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X961"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.2" customHeight="1"/>
@@ -2874,15 +2866,15 @@
       <c r="X1" s="80"/>
     </row>
     <row r="2" spans="1:24" ht="19.5" customHeight="1">
-      <c r="B2" s="131" t="s">
+      <c r="B2" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="133"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="138"/>
       <c r="I2" s="80"/>
       <c r="U2" s="80"/>
       <c r="V2" s="80"/>
@@ -2890,13 +2882,13 @@
       <c r="X2" s="80"/>
     </row>
     <row r="3" spans="1:24" ht="36" customHeight="1" thickBot="1">
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="136"/>
+      <c r="B3" s="139"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="141"/>
       <c r="I3" s="80"/>
       <c r="U3" s="80"/>
       <c r="V3" s="80"/>
@@ -2948,15 +2940,15 @@
       <c r="X6" s="80"/>
     </row>
     <row r="7" spans="1:24" ht="33.75" customHeight="1" thickBot="1">
-      <c r="B7" s="130" t="s">
-        <v>219</v>
-      </c>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="130"/>
-      <c r="H7" s="130"/>
+      <c r="B7" s="135" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="135"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
       <c r="I7" s="80"/>
       <c r="U7" s="82"/>
       <c r="V7" s="80"/>
@@ -2964,25 +2956,25 @@
       <c r="X7" s="80"/>
     </row>
     <row r="8" spans="1:24" ht="31.5" customHeight="1">
-      <c r="B8" s="234" t="s">
+      <c r="B8" s="236" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="235" t="s">
+      <c r="C8" s="237" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="236" t="s">
+      <c r="D8" s="238" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="237" t="s">
+      <c r="E8" s="239" t="s">
         <v>118</v>
       </c>
-      <c r="F8" s="238" t="s">
+      <c r="F8" s="240" t="s">
         <v>119</v>
       </c>
-      <c r="G8" s="239" t="s">
+      <c r="G8" s="241" t="s">
         <v>191</v>
       </c>
-      <c r="H8" s="240" t="s">
+      <c r="H8" s="242" t="s">
         <v>192</v>
       </c>
       <c r="U8" s="80"/>
@@ -3034,7 +3026,7 @@
       <c r="G10" s="83" t="s">
         <v>194</v>
       </c>
-      <c r="H10" s="231" t="s">
+      <c r="H10" s="127" t="s">
         <v>194</v>
       </c>
       <c r="U10" s="82"/>
@@ -3061,7 +3053,7 @@
       <c r="G11" s="83" t="s">
         <v>194</v>
       </c>
-      <c r="H11" s="231" t="s">
+      <c r="H11" s="127" t="s">
         <v>194</v>
       </c>
       <c r="U11" s="82"/>
@@ -3088,7 +3080,7 @@
       <c r="G12" s="118" t="s">
         <v>194</v>
       </c>
-      <c r="H12" s="232" t="s">
+      <c r="H12" s="128" t="s">
         <v>194</v>
       </c>
       <c r="U12" s="82"/>
@@ -3116,7 +3108,7 @@
     </row>
     <row r="14" spans="1:24" ht="40.5" customHeight="1" thickBot="1">
       <c r="B14" s="126" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C14" s="126"/>
       <c r="D14" s="126"/>
@@ -3142,25 +3134,25 @@
       <c r="X14" s="80"/>
     </row>
     <row r="15" spans="1:24" ht="32.25" customHeight="1">
-      <c r="B15" s="241" t="s">
+      <c r="B15" s="243" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="235" t="s">
+      <c r="C15" s="237" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="235" t="s">
+      <c r="D15" s="237" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="237" t="s">
-        <v>220</v>
-      </c>
-      <c r="F15" s="237" t="s">
+      <c r="E15" s="239" t="s">
+        <v>219</v>
+      </c>
+      <c r="F15" s="239" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="237" t="s">
+      <c r="G15" s="239" t="s">
         <v>79</v>
       </c>
-      <c r="H15" s="242" t="s">
+      <c r="H15" s="244" t="s">
         <v>82</v>
       </c>
       <c r="I15" s="80"/>
@@ -3181,7 +3173,7 @@
       <c r="X15" s="80"/>
     </row>
     <row r="16" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B16" s="127" t="s">
+      <c r="B16" s="132" t="s">
         <v>195</v>
       </c>
       <c r="C16" s="121" t="s">
@@ -3199,7 +3191,7 @@
       <c r="G16" s="111">
         <v>0</v>
       </c>
-      <c r="H16" s="233">
+      <c r="H16" s="129">
         <v>0</v>
       </c>
       <c r="I16" s="80"/>
@@ -3220,7 +3212,7 @@
       <c r="X16" s="80"/>
     </row>
     <row r="17" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B17" s="127"/>
+      <c r="B17" s="132"/>
       <c r="C17" s="122" t="s">
         <v>197</v>
       </c>
@@ -3236,7 +3228,7 @@
       <c r="G17" s="111">
         <v>0</v>
       </c>
-      <c r="H17" s="233">
+      <c r="H17" s="129">
         <v>0</v>
       </c>
       <c r="I17" s="80"/>
@@ -3257,7 +3249,7 @@
       <c r="X17" s="80"/>
     </row>
     <row r="18" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B18" s="127"/>
+      <c r="B18" s="132"/>
       <c r="C18" s="123" t="s">
         <v>198</v>
       </c>
@@ -3273,7 +3265,7 @@
       <c r="G18" s="111">
         <v>0</v>
       </c>
-      <c r="H18" s="233">
+      <c r="H18" s="129">
         <v>0</v>
       </c>
       <c r="I18" s="80"/>
@@ -3294,7 +3286,7 @@
       <c r="X18" s="80"/>
     </row>
     <row r="19" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B19" s="127"/>
+      <c r="B19" s="132"/>
       <c r="C19" s="123" t="s">
         <v>199</v>
       </c>
@@ -3310,7 +3302,7 @@
       <c r="G19" s="111">
         <v>0</v>
       </c>
-      <c r="H19" s="233">
+      <c r="H19" s="129">
         <v>0</v>
       </c>
       <c r="I19" s="80"/>
@@ -3331,7 +3323,7 @@
       <c r="X19" s="80"/>
     </row>
     <row r="20" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B20" s="127"/>
+      <c r="B20" s="132"/>
       <c r="C20" s="123" t="s">
         <v>200</v>
       </c>
@@ -3347,7 +3339,7 @@
       <c r="G20" s="111">
         <v>0</v>
       </c>
-      <c r="H20" s="233">
+      <c r="H20" s="129">
         <v>0</v>
       </c>
       <c r="I20" s="80"/>
@@ -3368,7 +3360,7 @@
       <c r="X20" s="80"/>
     </row>
     <row r="21" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B21" s="127"/>
+      <c r="B21" s="132"/>
       <c r="C21" s="123" t="s">
         <v>201</v>
       </c>
@@ -3384,7 +3376,7 @@
       <c r="G21" s="111">
         <v>0</v>
       </c>
-      <c r="H21" s="233">
+      <c r="H21" s="129">
         <v>0</v>
       </c>
       <c r="I21" s="80"/>
@@ -3394,7 +3386,7 @@
       <c r="X21" s="80"/>
     </row>
     <row r="22" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B22" s="127"/>
+      <c r="B22" s="132"/>
       <c r="C22" s="122" t="s">
         <v>202</v>
       </c>
@@ -3410,7 +3402,7 @@
       <c r="G22" s="111">
         <v>0</v>
       </c>
-      <c r="H22" s="233">
+      <c r="H22" s="129">
         <v>0</v>
       </c>
       <c r="I22" s="80"/>
@@ -3420,7 +3412,7 @@
       <c r="X22" s="80"/>
     </row>
     <row r="23" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B23" s="128" t="s">
+      <c r="B23" s="133" t="s">
         <v>203</v>
       </c>
       <c r="C23" s="120" t="s">
@@ -3438,7 +3430,7 @@
       <c r="G23" s="111">
         <v>0</v>
       </c>
-      <c r="H23" s="233">
+      <c r="H23" s="129">
         <v>0</v>
       </c>
       <c r="I23" s="80"/>
@@ -3448,7 +3440,7 @@
       <c r="X23" s="80"/>
     </row>
     <row r="24" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B24" s="128"/>
+      <c r="B24" s="133"/>
       <c r="C24" s="120" t="s">
         <v>205</v>
       </c>
@@ -3464,7 +3456,7 @@
       <c r="G24" s="111">
         <v>0</v>
       </c>
-      <c r="H24" s="233">
+      <c r="H24" s="129">
         <v>0</v>
       </c>
       <c r="I24" s="80"/>
@@ -3474,12 +3466,12 @@
       <c r="X24" s="80"/>
     </row>
     <row r="25" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B25" s="128"/>
+      <c r="B25" s="133"/>
       <c r="C25" s="120" t="s">
         <v>206</v>
       </c>
       <c r="D25" s="110" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E25" s="109" t="s">
         <v>120</v>
@@ -3490,7 +3482,7 @@
       <c r="G25" s="111">
         <v>0</v>
       </c>
-      <c r="H25" s="233">
+      <c r="H25" s="129">
         <v>0</v>
       </c>
       <c r="I25" s="80"/>
@@ -3500,7 +3492,7 @@
       <c r="X25" s="80"/>
     </row>
     <row r="26" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B26" s="128"/>
+      <c r="B26" s="133"/>
       <c r="C26" s="120" t="s">
         <v>207</v>
       </c>
@@ -3516,7 +3508,7 @@
       <c r="G26" s="111">
         <v>0</v>
       </c>
-      <c r="H26" s="233">
+      <c r="H26" s="129">
         <v>0</v>
       </c>
       <c r="I26" s="80"/>
@@ -3526,7 +3518,7 @@
       <c r="X26" s="80"/>
     </row>
     <row r="27" spans="1:24" ht="21.95" customHeight="1">
-      <c r="B27" s="128"/>
+      <c r="B27" s="133"/>
       <c r="C27" s="120" t="s">
         <v>208</v>
       </c>
@@ -3542,7 +3534,7 @@
       <c r="G27" s="111">
         <v>0</v>
       </c>
-      <c r="H27" s="233">
+      <c r="H27" s="129">
         <v>0</v>
       </c>
       <c r="I27" s="80"/>
@@ -3553,7 +3545,7 @@
     </row>
     <row r="28" spans="1:24" ht="21.95" customHeight="1" thickBot="1">
       <c r="A28" s="80"/>
-      <c r="B28" s="129"/>
+      <c r="B28" s="134"/>
       <c r="C28" s="124" t="s">
         <v>209</v>
       </c>
@@ -3563,13 +3555,13 @@
       <c r="E28" s="119" t="s">
         <v>120</v>
       </c>
-      <c r="F28" s="243">
+      <c r="F28" s="130">
         <v>0</v>
       </c>
-      <c r="G28" s="243">
+      <c r="G28" s="130">
         <v>0</v>
       </c>
-      <c r="H28" s="244">
+      <c r="H28" s="131">
         <v>0</v>
       </c>
       <c r="I28" s="80"/>
@@ -8873,23 +8865,23 @@
     </row>
     <row r="2" spans="1:36" ht="19.5" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="166" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="O2" s="138"/>
-      <c r="P2" s="138"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
+      <c r="P2" s="167"/>
       <c r="Q2" s="59"/>
       <c r="R2" s="60"/>
       <c r="S2" s="1"/>
@@ -8913,21 +8905,21 @@
     </row>
     <row r="3" spans="1:36" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="139"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="140"/>
-      <c r="O3" s="140"/>
-      <c r="P3" s="140"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
+      <c r="L3" s="169"/>
+      <c r="M3" s="169"/>
+      <c r="N3" s="169"/>
+      <c r="O3" s="169"/>
+      <c r="P3" s="169"/>
       <c r="Q3" s="61"/>
       <c r="R3" s="62"/>
       <c r="S3" s="1"/>
@@ -9083,12 +9075,12 @@
       <c r="E7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="141" t="s">
+      <c r="F7" s="170" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="141"/>
-      <c r="H7" s="141"/>
-      <c r="I7" s="141"/>
+      <c r="G7" s="170"/>
+      <c r="H7" s="170"/>
+      <c r="I7" s="170"/>
       <c r="J7" s="41" t="s">
         <v>76</v>
       </c>
@@ -9138,22 +9130,22 @@
       <c r="AJ7" s="1"/>
     </row>
     <row r="8" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A8" s="142"/>
-      <c r="B8" s="144" t="s">
+      <c r="A8" s="171"/>
+      <c r="B8" s="145" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="144" t="s">
+      <c r="C8" s="145" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="161"/>
-      <c r="E8" s="158" t="s">
+      <c r="D8" s="151"/>
+      <c r="E8" s="148" t="s">
         <v>53</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="20"/>
       <c r="I8" s="16"/>
-      <c r="J8" s="164" t="s">
+      <c r="J8" s="154" t="s">
         <v>100</v>
       </c>
       <c r="K8" s="57">
@@ -9194,16 +9186,16 @@
       <c r="AJ8" s="1"/>
     </row>
     <row r="9" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A9" s="142"/>
-      <c r="B9" s="145"/>
-      <c r="C9" s="145"/>
-      <c r="D9" s="162"/>
-      <c r="E9" s="159"/>
+      <c r="A9" s="171"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="146"/>
+      <c r="D9" s="152"/>
+      <c r="E9" s="149"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="20"/>
       <c r="I9" s="16"/>
-      <c r="J9" s="165"/>
+      <c r="J9" s="155"/>
       <c r="K9" s="57">
         <v>2</v>
       </c>
@@ -9242,16 +9234,16 @@
       <c r="AJ9" s="1"/>
     </row>
     <row r="10" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A10" s="142"/>
-      <c r="B10" s="145"/>
-      <c r="C10" s="146"/>
-      <c r="D10" s="163"/>
-      <c r="E10" s="160"/>
+      <c r="A10" s="171"/>
+      <c r="B10" s="146"/>
+      <c r="C10" s="147"/>
+      <c r="D10" s="153"/>
+      <c r="E10" s="150"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="16"/>
-      <c r="J10" s="166"/>
+      <c r="J10" s="156"/>
       <c r="K10" s="57">
         <v>3</v>
       </c>
@@ -9292,20 +9284,20 @@
       <c r="AJ10" s="1"/>
     </row>
     <row r="11" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A11" s="143"/>
-      <c r="B11" s="145"/>
-      <c r="C11" s="144" t="s">
+      <c r="A11" s="160"/>
+      <c r="B11" s="146"/>
+      <c r="C11" s="145" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="161"/>
-      <c r="E11" s="158" t="s">
+      <c r="D11" s="151"/>
+      <c r="E11" s="148" t="s">
         <v>72</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
       <c r="H11" s="29"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="164" t="s">
+      <c r="J11" s="154" t="s">
         <v>101</v>
       </c>
       <c r="K11" s="57">
@@ -9346,16 +9338,16 @@
       <c r="AJ11" s="1"/>
     </row>
     <row r="12" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A12" s="143"/>
-      <c r="B12" s="145"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="162"/>
-      <c r="E12" s="159"/>
+      <c r="A12" s="160"/>
+      <c r="B12" s="146"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="152"/>
+      <c r="E12" s="149"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="30"/>
-      <c r="J12" s="165"/>
+      <c r="J12" s="155"/>
       <c r="K12" s="57">
         <v>2</v>
       </c>
@@ -9394,16 +9386,16 @@
       <c r="AJ12" s="1"/>
     </row>
     <row r="13" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A13" s="143"/>
-      <c r="B13" s="145"/>
-      <c r="C13" s="146"/>
-      <c r="D13" s="163"/>
-      <c r="E13" s="160"/>
+      <c r="A13" s="160"/>
+      <c r="B13" s="146"/>
+      <c r="C13" s="147"/>
+      <c r="D13" s="153"/>
+      <c r="E13" s="150"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
       <c r="I13" s="30"/>
-      <c r="J13" s="166"/>
+      <c r="J13" s="156"/>
       <c r="K13" s="57">
         <v>3</v>
       </c>
@@ -9438,20 +9430,20 @@
       <c r="AJ13" s="1"/>
     </row>
     <row r="14" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A14" s="143"/>
-      <c r="B14" s="145"/>
-      <c r="C14" s="144" t="s">
+      <c r="A14" s="160"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="161"/>
-      <c r="E14" s="158" t="s">
+      <c r="D14" s="151"/>
+      <c r="E14" s="148" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
       <c r="H14" s="29"/>
       <c r="I14" s="30"/>
-      <c r="J14" s="169" t="s">
+      <c r="J14" s="159" t="s">
         <v>102</v>
       </c>
       <c r="K14" s="57">
@@ -9492,16 +9484,16 @@
       <c r="AJ14" s="1"/>
     </row>
     <row r="15" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A15" s="143"/>
-      <c r="B15" s="145"/>
-      <c r="C15" s="145"/>
-      <c r="D15" s="162"/>
-      <c r="E15" s="159"/>
+      <c r="A15" s="160"/>
+      <c r="B15" s="146"/>
+      <c r="C15" s="146"/>
+      <c r="D15" s="152"/>
+      <c r="E15" s="149"/>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
       <c r="I15" s="30"/>
-      <c r="J15" s="165"/>
+      <c r="J15" s="155"/>
       <c r="K15" s="57">
         <v>2</v>
       </c>
@@ -9540,16 +9532,16 @@
       <c r="AJ15" s="1"/>
     </row>
     <row r="16" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A16" s="143"/>
-      <c r="B16" s="146"/>
-      <c r="C16" s="146"/>
-      <c r="D16" s="167"/>
-      <c r="E16" s="168"/>
+      <c r="A16" s="160"/>
+      <c r="B16" s="147"/>
+      <c r="C16" s="147"/>
+      <c r="D16" s="157"/>
+      <c r="E16" s="158"/>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
       <c r="I16" s="30"/>
-      <c r="J16" s="166"/>
+      <c r="J16" s="156"/>
       <c r="K16" s="57">
         <v>3</v>
       </c>
@@ -9592,22 +9584,22 @@
       <c r="AJ16" s="1"/>
     </row>
     <row r="17" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A17" s="142"/>
-      <c r="B17" s="144" t="s">
+      <c r="A17" s="171"/>
+      <c r="B17" s="145" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="144" t="s">
+      <c r="C17" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="151"/>
-      <c r="E17" s="143" t="s">
+      <c r="D17" s="163"/>
+      <c r="E17" s="160" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="45"/>
-      <c r="J17" s="147" t="s">
+      <c r="J17" s="172" t="s">
         <v>103</v>
       </c>
       <c r="K17" s="57">
@@ -9640,16 +9632,16 @@
       <c r="AJ17" s="1"/>
     </row>
     <row r="18" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A18" s="142"/>
-      <c r="B18" s="145"/>
-      <c r="C18" s="145"/>
-      <c r="D18" s="152"/>
-      <c r="E18" s="150"/>
+      <c r="A18" s="171"/>
+      <c r="B18" s="146"/>
+      <c r="C18" s="146"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="161"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="45"/>
-      <c r="J18" s="148"/>
+      <c r="J18" s="173"/>
       <c r="K18" s="57">
         <v>2</v>
       </c>
@@ -9680,16 +9672,16 @@
       <c r="AJ18" s="1"/>
     </row>
     <row r="19" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A19" s="142"/>
-      <c r="B19" s="145"/>
-      <c r="C19" s="145"/>
-      <c r="D19" s="152"/>
-      <c r="E19" s="150"/>
+      <c r="A19" s="171"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="146"/>
+      <c r="D19" s="164"/>
+      <c r="E19" s="161"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="45"/>
-      <c r="J19" s="148"/>
+      <c r="J19" s="173"/>
       <c r="K19" s="57">
         <v>3</v>
       </c>
@@ -9720,16 +9712,16 @@
       <c r="AJ19" s="1"/>
     </row>
     <row r="20" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A20" s="142"/>
-      <c r="B20" s="145"/>
-      <c r="C20" s="145"/>
-      <c r="D20" s="152"/>
-      <c r="E20" s="150"/>
+      <c r="A20" s="171"/>
+      <c r="B20" s="146"/>
+      <c r="C20" s="146"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="161"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
       <c r="I20" s="45"/>
-      <c r="J20" s="148"/>
+      <c r="J20" s="173"/>
       <c r="K20" s="57">
         <v>4</v>
       </c>
@@ -9760,16 +9752,16 @@
       <c r="AJ20" s="1"/>
     </row>
     <row r="21" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A21" s="142"/>
-      <c r="B21" s="145"/>
-      <c r="C21" s="145"/>
-      <c r="D21" s="152"/>
-      <c r="E21" s="150"/>
+      <c r="A21" s="171"/>
+      <c r="B21" s="146"/>
+      <c r="C21" s="146"/>
+      <c r="D21" s="164"/>
+      <c r="E21" s="161"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
       <c r="I21" s="45"/>
-      <c r="J21" s="148"/>
+      <c r="J21" s="173"/>
       <c r="K21" s="57">
         <v>5</v>
       </c>
@@ -9800,16 +9792,16 @@
       <c r="AJ21" s="1"/>
     </row>
     <row r="22" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A22" s="142"/>
-      <c r="B22" s="145"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="154"/>
-      <c r="E22" s="153"/>
+      <c r="A22" s="171"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="147"/>
+      <c r="D22" s="165"/>
+      <c r="E22" s="162"/>
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
       <c r="I22" s="46"/>
-      <c r="J22" s="149"/>
+      <c r="J22" s="174"/>
       <c r="K22" s="58">
         <v>6</v>
       </c>
@@ -9840,20 +9832,20 @@
       <c r="AJ22" s="1"/>
     </row>
     <row r="23" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A23" s="142"/>
-      <c r="B23" s="145"/>
-      <c r="C23" s="144" t="s">
+      <c r="A23" s="171"/>
+      <c r="B23" s="146"/>
+      <c r="C23" s="145" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="151"/>
-      <c r="E23" s="143" t="s">
+      <c r="D23" s="163"/>
+      <c r="E23" s="160" t="s">
         <v>72</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
       <c r="I23" s="46"/>
-      <c r="J23" s="147" t="s">
+      <c r="J23" s="172" t="s">
         <v>104</v>
       </c>
       <c r="K23" s="58">
@@ -9886,16 +9878,16 @@
       <c r="AJ23" s="1"/>
     </row>
     <row r="24" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A24" s="142"/>
-      <c r="B24" s="145"/>
-      <c r="C24" s="145"/>
-      <c r="D24" s="152"/>
-      <c r="E24" s="150"/>
+      <c r="A24" s="171"/>
+      <c r="B24" s="146"/>
+      <c r="C24" s="146"/>
+      <c r="D24" s="164"/>
+      <c r="E24" s="161"/>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
       <c r="I24" s="46"/>
-      <c r="J24" s="148"/>
+      <c r="J24" s="173"/>
       <c r="K24" s="58">
         <v>2</v>
       </c>
@@ -9926,16 +9918,16 @@
       <c r="AJ24" s="1"/>
     </row>
     <row r="25" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A25" s="142"/>
-      <c r="B25" s="145"/>
-      <c r="C25" s="145"/>
-      <c r="D25" s="152"/>
-      <c r="E25" s="150"/>
+      <c r="A25" s="171"/>
+      <c r="B25" s="146"/>
+      <c r="C25" s="146"/>
+      <c r="D25" s="164"/>
+      <c r="E25" s="161"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
       <c r="I25" s="46"/>
-      <c r="J25" s="148"/>
+      <c r="J25" s="173"/>
       <c r="K25" s="58">
         <v>3</v>
       </c>
@@ -9966,16 +9958,16 @@
       <c r="AJ25" s="1"/>
     </row>
     <row r="26" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A26" s="142"/>
-      <c r="B26" s="145"/>
-      <c r="C26" s="145"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="150"/>
+      <c r="A26" s="171"/>
+      <c r="B26" s="146"/>
+      <c r="C26" s="146"/>
+      <c r="D26" s="164"/>
+      <c r="E26" s="161"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
       <c r="I26" s="46"/>
-      <c r="J26" s="148"/>
+      <c r="J26" s="173"/>
       <c r="K26" s="58">
         <v>4</v>
       </c>
@@ -10006,16 +9998,16 @@
       <c r="AJ26" s="1"/>
     </row>
     <row r="27" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A27" s="142"/>
-      <c r="B27" s="145"/>
-      <c r="C27" s="145"/>
-      <c r="D27" s="152"/>
-      <c r="E27" s="150"/>
+      <c r="A27" s="171"/>
+      <c r="B27" s="146"/>
+      <c r="C27" s="146"/>
+      <c r="D27" s="164"/>
+      <c r="E27" s="161"/>
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
       <c r="I27" s="46"/>
-      <c r="J27" s="148"/>
+      <c r="J27" s="173"/>
       <c r="K27" s="58">
         <v>5</v>
       </c>
@@ -10046,16 +10038,16 @@
       <c r="AJ27" s="1"/>
     </row>
     <row r="28" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A28" s="142"/>
-      <c r="B28" s="145"/>
-      <c r="C28" s="145"/>
-      <c r="D28" s="152"/>
-      <c r="E28" s="150"/>
+      <c r="A28" s="171"/>
+      <c r="B28" s="146"/>
+      <c r="C28" s="146"/>
+      <c r="D28" s="164"/>
+      <c r="E28" s="161"/>
       <c r="F28" s="69"/>
       <c r="G28" s="69"/>
       <c r="H28" s="69"/>
       <c r="I28" s="70"/>
-      <c r="J28" s="148"/>
+      <c r="J28" s="173"/>
       <c r="K28" s="58">
         <v>6</v>
       </c>
@@ -10086,20 +10078,20 @@
       <c r="AJ28" s="1"/>
     </row>
     <row r="29" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A29" s="142"/>
-      <c r="B29" s="145"/>
-      <c r="C29" s="144" t="s">
+      <c r="A29" s="171"/>
+      <c r="B29" s="146"/>
+      <c r="C29" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="151"/>
-      <c r="E29" s="143" t="s">
+      <c r="D29" s="163"/>
+      <c r="E29" s="160" t="s">
         <v>54</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
       <c r="H29" s="27"/>
       <c r="I29" s="46"/>
-      <c r="J29" s="147" t="s">
+      <c r="J29" s="172" t="s">
         <v>105</v>
       </c>
       <c r="K29" s="58">
@@ -10132,16 +10124,16 @@
       <c r="AJ29" s="1"/>
     </row>
     <row r="30" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A30" s="142"/>
-      <c r="B30" s="145"/>
-      <c r="C30" s="145"/>
-      <c r="D30" s="152"/>
-      <c r="E30" s="150"/>
+      <c r="A30" s="171"/>
+      <c r="B30" s="146"/>
+      <c r="C30" s="146"/>
+      <c r="D30" s="164"/>
+      <c r="E30" s="161"/>
       <c r="F30" s="27"/>
       <c r="G30" s="27"/>
       <c r="H30" s="27"/>
       <c r="I30" s="46"/>
-      <c r="J30" s="148"/>
+      <c r="J30" s="173"/>
       <c r="K30" s="58">
         <v>2</v>
       </c>
@@ -10172,16 +10164,16 @@
       <c r="AJ30" s="1"/>
     </row>
     <row r="31" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A31" s="142"/>
-      <c r="B31" s="145"/>
-      <c r="C31" s="145"/>
-      <c r="D31" s="152"/>
-      <c r="E31" s="150"/>
+      <c r="A31" s="171"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="164"/>
+      <c r="E31" s="161"/>
       <c r="F31" s="27"/>
       <c r="G31" s="27"/>
       <c r="H31" s="27"/>
       <c r="I31" s="46"/>
-      <c r="J31" s="148"/>
+      <c r="J31" s="173"/>
       <c r="K31" s="58">
         <v>3</v>
       </c>
@@ -10212,16 +10204,16 @@
       <c r="AJ31" s="1"/>
     </row>
     <row r="32" spans="1:36" ht="16.5" customHeight="1">
-      <c r="A32" s="142"/>
-      <c r="B32" s="146"/>
-      <c r="C32" s="146"/>
-      <c r="D32" s="154"/>
-      <c r="E32" s="153"/>
+      <c r="A32" s="171"/>
+      <c r="B32" s="147"/>
+      <c r="C32" s="147"/>
+      <c r="D32" s="165"/>
+      <c r="E32" s="162"/>
       <c r="F32" s="27"/>
       <c r="G32" s="27"/>
       <c r="H32" s="27"/>
       <c r="I32" s="46"/>
-      <c r="J32" s="149"/>
+      <c r="J32" s="174"/>
       <c r="K32" s="58">
         <v>4</v>
       </c>
@@ -10253,7 +10245,7 @@
     </row>
     <row r="33" spans="1:36" ht="16.149999999999999" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="155" t="s">
+      <c r="B33" s="142" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="38" t="s">
@@ -10295,7 +10287,7 @@
     </row>
     <row r="34" spans="1:36" ht="16.149999999999999" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="156"/>
+      <c r="B34" s="143"/>
       <c r="C34" s="38" t="s">
         <v>64</v>
       </c>
@@ -10335,7 +10327,7 @@
     </row>
     <row r="35" spans="1:36" ht="16.149999999999999" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="156"/>
+      <c r="B35" s="143"/>
       <c r="C35" s="38" t="s">
         <v>57</v>
       </c>
@@ -10375,7 +10367,7 @@
     </row>
     <row r="36" spans="1:36" ht="16.149999999999999" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="157"/>
+      <c r="B36" s="144"/>
       <c r="C36" s="38" t="s">
         <v>66</v>
       </c>
@@ -18551,6 +18543,21 @@
     <filterColumn colId="8" hiddenButton="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="31">
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A17:A32"/>
+    <mergeCell ref="B8:B16"/>
+    <mergeCell ref="B17:B32"/>
+    <mergeCell ref="J17:J22"/>
+    <mergeCell ref="C23:C28"/>
+    <mergeCell ref="J23:J28"/>
+    <mergeCell ref="E23:E28"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="J29:J32"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="C29:C32"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="E8:E10"/>
@@ -18567,21 +18574,6 @@
     <mergeCell ref="C17:C22"/>
     <mergeCell ref="E17:E22"/>
     <mergeCell ref="D17:D22"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="A17:A32"/>
-    <mergeCell ref="B8:B16"/>
-    <mergeCell ref="B17:B32"/>
-    <mergeCell ref="J17:J22"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="J23:J28"/>
-    <mergeCell ref="E23:E28"/>
-    <mergeCell ref="D23:D28"/>
-    <mergeCell ref="J29:J32"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="C29:C32"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -18659,24 +18651,24 @@
     </row>
     <row r="2" spans="1:37" ht="19.5" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="166" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="O2" s="138"/>
-      <c r="P2" s="138"/>
-      <c r="Q2" s="138"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
+      <c r="P2" s="167"/>
+      <c r="Q2" s="167"/>
       <c r="R2" s="59"/>
       <c r="S2" s="60"/>
       <c r="T2" s="1"/>
@@ -18700,22 +18692,22 @@
     </row>
     <row r="3" spans="1:37" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="139"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="140"/>
-      <c r="O3" s="140"/>
-      <c r="P3" s="140"/>
-      <c r="Q3" s="140"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
+      <c r="L3" s="169"/>
+      <c r="M3" s="169"/>
+      <c r="N3" s="169"/>
+      <c r="O3" s="169"/>
+      <c r="P3" s="169"/>
+      <c r="Q3" s="169"/>
       <c r="R3" s="61"/>
       <c r="S3" s="62"/>
       <c r="T3" s="1"/>
@@ -18874,12 +18866,12 @@
       <c r="E7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="190" t="s">
+      <c r="F7" s="175" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="191"/>
-      <c r="H7" s="191"/>
-      <c r="I7" s="192"/>
+      <c r="G7" s="176"/>
+      <c r="H7" s="176"/>
+      <c r="I7" s="177"/>
       <c r="J7" s="97" t="s">
         <v>76</v>
       </c>
@@ -18932,27 +18924,27 @@
       <c r="AK7" s="1"/>
     </row>
     <row r="8" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A8" s="143" t="s">
+      <c r="A8" s="160" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="174" t="s">
+      <c r="B8" s="186" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="177" t="s">
+      <c r="C8" s="205" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="193"/>
-      <c r="E8" s="196" t="s">
+      <c r="D8" s="180"/>
+      <c r="E8" s="183" t="s">
         <v>44</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="15"/>
-      <c r="J8" s="164" t="s">
+      <c r="J8" s="154" t="s">
         <v>96</v>
       </c>
-      <c r="K8" s="164">
+      <c r="K8" s="154">
         <v>1</v>
       </c>
       <c r="L8" s="57">
@@ -18993,17 +18985,17 @@
       <c r="AK8" s="1"/>
     </row>
     <row r="9" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A9" s="150"/>
-      <c r="B9" s="175"/>
-      <c r="C9" s="178"/>
-      <c r="D9" s="194"/>
+      <c r="A9" s="161"/>
+      <c r="B9" s="187"/>
+      <c r="C9" s="206"/>
+      <c r="D9" s="181"/>
       <c r="E9" s="184"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="15"/>
-      <c r="J9" s="180"/>
-      <c r="K9" s="180"/>
+      <c r="J9" s="178"/>
+      <c r="K9" s="178"/>
       <c r="L9" s="57">
         <v>2</v>
       </c>
@@ -19042,17 +19034,17 @@
       <c r="AK9" s="1"/>
     </row>
     <row r="10" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A10" s="150"/>
-      <c r="B10" s="175"/>
-      <c r="C10" s="178"/>
-      <c r="D10" s="194"/>
+      <c r="A10" s="161"/>
+      <c r="B10" s="187"/>
+      <c r="C10" s="206"/>
+      <c r="D10" s="181"/>
       <c r="E10" s="184"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="16"/>
-      <c r="J10" s="180"/>
-      <c r="K10" s="180"/>
+      <c r="J10" s="178"/>
+      <c r="K10" s="178"/>
       <c r="L10" s="57">
         <v>3</v>
       </c>
@@ -19097,17 +19089,17 @@
       <c r="AK10" s="1"/>
     </row>
     <row r="11" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A11" s="150"/>
-      <c r="B11" s="175"/>
-      <c r="C11" s="178"/>
-      <c r="D11" s="194"/>
+      <c r="A11" s="161"/>
+      <c r="B11" s="187"/>
+      <c r="C11" s="206"/>
+      <c r="D11" s="181"/>
       <c r="E11" s="184"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="16"/>
-      <c r="J11" s="180"/>
-      <c r="K11" s="180"/>
+      <c r="J11" s="178"/>
+      <c r="K11" s="178"/>
       <c r="L11" s="57">
         <v>4</v>
       </c>
@@ -19117,8 +19109,8 @@
       <c r="N11" s="72" t="s">
         <v>172</v>
       </c>
-      <c r="O11" s="198"/>
-      <c r="P11" s="199"/>
+      <c r="O11" s="190"/>
+      <c r="P11" s="191"/>
       <c r="Q11" s="75"/>
       <c r="R11" s="7"/>
       <c r="S11" s="8"/>
@@ -19142,17 +19134,17 @@
       <c r="AK11" s="1"/>
     </row>
     <row r="12" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A12" s="150"/>
-      <c r="B12" s="175"/>
-      <c r="C12" s="178"/>
-      <c r="D12" s="194"/>
+      <c r="A12" s="161"/>
+      <c r="B12" s="187"/>
+      <c r="C12" s="206"/>
+      <c r="D12" s="181"/>
       <c r="E12" s="184"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="16"/>
-      <c r="J12" s="180"/>
-      <c r="K12" s="180"/>
+      <c r="J12" s="178"/>
+      <c r="K12" s="178"/>
       <c r="L12" s="57">
         <v>5</v>
       </c>
@@ -19162,8 +19154,8 @@
       <c r="N12" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="O12" s="200"/>
-      <c r="P12" s="201"/>
+      <c r="O12" s="192"/>
+      <c r="P12" s="193"/>
       <c r="Q12" s="75"/>
       <c r="R12" s="7"/>
       <c r="S12" s="8"/>
@@ -19187,17 +19179,17 @@
       <c r="AK12" s="1"/>
     </row>
     <row r="13" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A13" s="150"/>
-      <c r="B13" s="175"/>
-      <c r="C13" s="178"/>
-      <c r="D13" s="194"/>
+      <c r="A13" s="161"/>
+      <c r="B13" s="187"/>
+      <c r="C13" s="206"/>
+      <c r="D13" s="181"/>
       <c r="E13" s="184"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="16"/>
-      <c r="J13" s="180"/>
-      <c r="K13" s="180"/>
+      <c r="J13" s="178"/>
+      <c r="K13" s="178"/>
       <c r="L13" s="57">
         <v>6</v>
       </c>
@@ -19207,8 +19199,8 @@
       <c r="N13" s="72" t="s">
         <v>171</v>
       </c>
-      <c r="O13" s="200"/>
-      <c r="P13" s="201"/>
+      <c r="O13" s="192"/>
+      <c r="P13" s="193"/>
       <c r="Q13" s="75"/>
       <c r="R13" s="7"/>
       <c r="S13" s="8"/>
@@ -19232,17 +19224,17 @@
       <c r="AK13" s="1"/>
     </row>
     <row r="14" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A14" s="150"/>
-      <c r="B14" s="175"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="195"/>
+      <c r="A14" s="161"/>
+      <c r="B14" s="187"/>
+      <c r="C14" s="207"/>
+      <c r="D14" s="182"/>
       <c r="E14" s="185"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="181"/>
-      <c r="K14" s="181"/>
+      <c r="J14" s="179"/>
+      <c r="K14" s="179"/>
       <c r="L14" s="57">
         <v>7</v>
       </c>
@@ -19252,8 +19244,8 @@
       <c r="N14" s="72" t="s">
         <v>171</v>
       </c>
-      <c r="O14" s="202"/>
-      <c r="P14" s="203"/>
+      <c r="O14" s="194"/>
+      <c r="P14" s="195"/>
       <c r="Q14" s="75"/>
       <c r="R14" s="7"/>
       <c r="S14" s="8"/>
@@ -19277,8 +19269,8 @@
       <c r="AK14" s="1"/>
     </row>
     <row r="15" spans="1:37" ht="26.25" customHeight="1">
-      <c r="A15" s="150"/>
-      <c r="B15" s="176"/>
+      <c r="A15" s="161"/>
+      <c r="B15" s="188"/>
       <c r="C15" s="102" t="s">
         <v>133</v>
       </c>
@@ -19334,25 +19326,25 @@
       <c r="AK15" s="1"/>
     </row>
     <row r="16" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A16" s="150"/>
-      <c r="B16" s="174" t="s">
+      <c r="A16" s="161"/>
+      <c r="B16" s="186" t="s">
         <v>134</v>
       </c>
-      <c r="C16" s="177" t="s">
+      <c r="C16" s="205" t="s">
         <v>135</v>
       </c>
-      <c r="D16" s="197"/>
-      <c r="E16" s="183" t="s">
+      <c r="D16" s="189"/>
+      <c r="E16" s="199" t="s">
         <v>44</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="16"/>
-      <c r="J16" s="164" t="s">
+      <c r="J16" s="154" t="s">
         <v>139</v>
       </c>
-      <c r="K16" s="169">
+      <c r="K16" s="159">
         <v>3</v>
       </c>
       <c r="L16" s="57">
@@ -19393,17 +19385,17 @@
       <c r="AK16" s="1"/>
     </row>
     <row r="17" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A17" s="150"/>
-      <c r="B17" s="175"/>
-      <c r="C17" s="178"/>
-      <c r="D17" s="194"/>
+      <c r="A17" s="161"/>
+      <c r="B17" s="187"/>
+      <c r="C17" s="206"/>
+      <c r="D17" s="181"/>
       <c r="E17" s="184"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="16"/>
-      <c r="J17" s="180"/>
-      <c r="K17" s="165"/>
+      <c r="J17" s="178"/>
+      <c r="K17" s="155"/>
       <c r="L17" s="57">
         <v>2</v>
       </c>
@@ -19442,17 +19434,17 @@
       <c r="AK17" s="1"/>
     </row>
     <row r="18" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A18" s="150"/>
-      <c r="B18" s="175"/>
-      <c r="C18" s="179"/>
-      <c r="D18" s="194"/>
+      <c r="A18" s="161"/>
+      <c r="B18" s="187"/>
+      <c r="C18" s="207"/>
+      <c r="D18" s="181"/>
       <c r="E18" s="184"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="16"/>
-      <c r="J18" s="181"/>
-      <c r="K18" s="165"/>
+      <c r="J18" s="179"/>
+      <c r="K18" s="155"/>
       <c r="L18" s="57">
         <v>3</v>
       </c>
@@ -19491,21 +19483,21 @@
       <c r="AK18" s="1"/>
     </row>
     <row r="19" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A19" s="150"/>
-      <c r="B19" s="175"/>
-      <c r="C19" s="177" t="s">
+      <c r="A19" s="161"/>
+      <c r="B19" s="187"/>
+      <c r="C19" s="205" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="194"/>
+      <c r="D19" s="181"/>
       <c r="E19" s="184"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="16"/>
-      <c r="J19" s="164" t="s">
+      <c r="J19" s="154" t="s">
         <v>140</v>
       </c>
-      <c r="K19" s="165"/>
+      <c r="K19" s="155"/>
       <c r="L19" s="57">
         <v>4</v>
       </c>
@@ -19544,17 +19536,17 @@
       <c r="AK19" s="1"/>
     </row>
     <row r="20" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A20" s="150"/>
-      <c r="B20" s="175"/>
-      <c r="C20" s="179"/>
-      <c r="D20" s="194"/>
+      <c r="A20" s="161"/>
+      <c r="B20" s="187"/>
+      <c r="C20" s="207"/>
+      <c r="D20" s="181"/>
       <c r="E20" s="184"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="16"/>
-      <c r="J20" s="181"/>
-      <c r="K20" s="165"/>
+      <c r="J20" s="179"/>
+      <c r="K20" s="155"/>
       <c r="L20" s="57">
         <v>5</v>
       </c>
@@ -19599,12 +19591,12 @@
       <c r="AK20" s="1"/>
     </row>
     <row r="21" spans="1:37" ht="32.25" customHeight="1">
-      <c r="A21" s="150"/>
-      <c r="B21" s="175"/>
+      <c r="A21" s="161"/>
+      <c r="B21" s="187"/>
       <c r="C21" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="194"/>
+      <c r="D21" s="181"/>
       <c r="E21" s="184"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -19613,7 +19605,7 @@
       <c r="J21" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="K21" s="165"/>
+      <c r="K21" s="155"/>
       <c r="L21" s="57">
         <v>6</v>
       </c>
@@ -19652,21 +19644,21 @@
       <c r="AK21" s="1"/>
     </row>
     <row r="22" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A22" s="150"/>
-      <c r="B22" s="175"/>
-      <c r="C22" s="177" t="s">
+      <c r="A22" s="161"/>
+      <c r="B22" s="187"/>
+      <c r="C22" s="205" t="s">
         <v>138</v>
       </c>
-      <c r="D22" s="194"/>
+      <c r="D22" s="181"/>
       <c r="E22" s="184"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="16"/>
-      <c r="J22" s="164" t="s">
+      <c r="J22" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="K22" s="165"/>
+      <c r="K22" s="155"/>
       <c r="L22" s="57">
         <v>7</v>
       </c>
@@ -19705,17 +19697,17 @@
       <c r="AK22" s="1"/>
     </row>
     <row r="23" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A23" s="150"/>
-      <c r="B23" s="176"/>
-      <c r="C23" s="179"/>
-      <c r="D23" s="195"/>
+      <c r="A23" s="161"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="207"/>
+      <c r="D23" s="182"/>
       <c r="E23" s="185"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="16"/>
-      <c r="J23" s="181"/>
-      <c r="K23" s="166"/>
+      <c r="J23" s="179"/>
+      <c r="K23" s="156"/>
       <c r="L23" s="57">
         <v>8</v>
       </c>
@@ -19754,25 +19746,25 @@
       <c r="AK23" s="1"/>
     </row>
     <row r="24" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A24" s="150"/>
-      <c r="B24" s="186" t="s">
+      <c r="A24" s="161"/>
+      <c r="B24" s="196" t="s">
         <v>162</v>
       </c>
-      <c r="C24" s="174" t="s">
+      <c r="C24" s="186" t="s">
         <v>163</v>
       </c>
-      <c r="D24" s="161"/>
-      <c r="E24" s="183" t="s">
+      <c r="D24" s="151"/>
+      <c r="E24" s="199" t="s">
         <v>44</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="16"/>
-      <c r="J24" s="164" t="s">
+      <c r="J24" s="154" t="s">
         <v>98</v>
       </c>
-      <c r="K24" s="164">
+      <c r="K24" s="154">
         <v>2</v>
       </c>
       <c r="L24" s="57">
@@ -19813,17 +19805,17 @@
       <c r="AK24" s="1"/>
     </row>
     <row r="25" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A25" s="150"/>
-      <c r="B25" s="187"/>
-      <c r="C25" s="175"/>
-      <c r="D25" s="162"/>
+      <c r="A25" s="161"/>
+      <c r="B25" s="197"/>
+      <c r="C25" s="187"/>
+      <c r="D25" s="152"/>
       <c r="E25" s="184"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="16"/>
-      <c r="J25" s="180"/>
-      <c r="K25" s="180"/>
+      <c r="J25" s="178"/>
+      <c r="K25" s="178"/>
       <c r="L25" s="57">
         <v>2</v>
       </c>
@@ -19862,17 +19854,17 @@
       <c r="AK25" s="1"/>
     </row>
     <row r="26" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A26" s="150"/>
-      <c r="B26" s="187"/>
-      <c r="C26" s="176"/>
-      <c r="D26" s="162"/>
+      <c r="A26" s="161"/>
+      <c r="B26" s="197"/>
+      <c r="C26" s="188"/>
+      <c r="D26" s="152"/>
       <c r="E26" s="184"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="16"/>
-      <c r="J26" s="181"/>
-      <c r="K26" s="181"/>
+      <c r="J26" s="179"/>
+      <c r="K26" s="179"/>
       <c r="L26" s="57">
         <v>3</v>
       </c>
@@ -19911,13 +19903,13 @@
       <c r="AK26" s="1"/>
     </row>
     <row r="27" spans="1:37" ht="38.25" customHeight="1">
-      <c r="A27" s="153"/>
-      <c r="B27" s="188"/>
+      <c r="A27" s="162"/>
+      <c r="B27" s="198"/>
       <c r="C27" s="104" t="s">
         <v>164</v>
       </c>
-      <c r="D27" s="163"/>
-      <c r="E27" s="189"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="200"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -19966,27 +19958,27 @@
       <c r="AK27" s="1"/>
     </row>
     <row r="28" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A28" s="143" t="s">
+      <c r="A28" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="174" t="s">
+      <c r="B28" s="186" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="182"/>
-      <c r="E28" s="143" t="s">
+      <c r="D28" s="208"/>
+      <c r="E28" s="160" t="s">
         <v>44</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
       <c r="H28" s="17"/>
       <c r="I28" s="45"/>
-      <c r="J28" s="147" t="s">
+      <c r="J28" s="172" t="s">
         <v>130</v>
       </c>
-      <c r="K28" s="164">
+      <c r="K28" s="154">
         <v>4</v>
       </c>
       <c r="L28" s="57">
@@ -19998,8 +19990,8 @@
       <c r="N28" s="73" t="s">
         <v>129</v>
       </c>
-      <c r="O28" s="170"/>
-      <c r="P28" s="171"/>
+      <c r="O28" s="201"/>
+      <c r="P28" s="202"/>
       <c r="Q28" s="77"/>
       <c r="R28" s="18"/>
       <c r="S28" s="2"/>
@@ -20023,19 +20015,19 @@
       <c r="AK28" s="1"/>
     </row>
     <row r="29" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A29" s="150"/>
-      <c r="B29" s="175"/>
+      <c r="A29" s="161"/>
+      <c r="B29" s="187"/>
       <c r="C29" s="89" t="s">
         <v>145</v>
       </c>
-      <c r="D29" s="152"/>
-      <c r="E29" s="150"/>
+      <c r="D29" s="164"/>
+      <c r="E29" s="161"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
       <c r="I29" s="45"/>
-      <c r="J29" s="148"/>
-      <c r="K29" s="180"/>
+      <c r="J29" s="173"/>
+      <c r="K29" s="178"/>
       <c r="L29" s="57">
         <v>2</v>
       </c>
@@ -20045,8 +20037,8 @@
       <c r="N29" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="O29" s="172"/>
-      <c r="P29" s="173"/>
+      <c r="O29" s="203"/>
+      <c r="P29" s="204"/>
       <c r="Q29" s="77"/>
       <c r="R29" s="66"/>
       <c r="S29" s="2"/>
@@ -20070,19 +20062,19 @@
       <c r="AK29" s="1"/>
     </row>
     <row r="30" spans="1:37" ht="19.5" customHeight="1">
-      <c r="A30" s="150"/>
-      <c r="B30" s="176"/>
+      <c r="A30" s="161"/>
+      <c r="B30" s="188"/>
       <c r="C30" s="99" t="s">
         <v>146</v>
       </c>
-      <c r="D30" s="154"/>
-      <c r="E30" s="153"/>
+      <c r="D30" s="165"/>
+      <c r="E30" s="162"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
       <c r="I30" s="45"/>
-      <c r="J30" s="149"/>
-      <c r="K30" s="181"/>
+      <c r="J30" s="174"/>
+      <c r="K30" s="179"/>
       <c r="L30" s="57">
         <v>3</v>
       </c>
@@ -20092,8 +20084,8 @@
       <c r="N30" s="73" t="s">
         <v>129</v>
       </c>
-      <c r="O30" s="172"/>
-      <c r="P30" s="173"/>
+      <c r="O30" s="203"/>
+      <c r="P30" s="204"/>
       <c r="Q30" s="77"/>
       <c r="R30" s="66"/>
       <c r="S30" s="2"/>
@@ -20117,7 +20109,7 @@
       <c r="AK30" s="1"/>
     </row>
     <row r="31" spans="1:37" ht="32.25" customHeight="1">
-      <c r="A31" s="153"/>
+      <c r="A31" s="162"/>
       <c r="B31" s="89" t="s">
         <v>147</v>
       </c>
@@ -20147,8 +20139,8 @@
       <c r="N31" s="73" t="s">
         <v>129</v>
       </c>
-      <c r="O31" s="172"/>
-      <c r="P31" s="173"/>
+      <c r="O31" s="203"/>
+      <c r="P31" s="204"/>
       <c r="Q31" s="77"/>
       <c r="R31" s="66"/>
       <c r="S31" s="2"/>
@@ -28678,6 +28670,25 @@
     <filterColumn colId="8" hiddenButton="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="33">
+    <mergeCell ref="O28:P31"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C8:C14"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="E16:E23"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="C24:C26"/>
     <mergeCell ref="B2:Q3"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="A8:A27"/>
@@ -28692,25 +28703,6 @@
     <mergeCell ref="K16:K23"/>
     <mergeCell ref="D16:D23"/>
     <mergeCell ref="O11:P14"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="O28:P31"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C8:C14"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="E16:E23"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -28788,24 +28780,24 @@
     </row>
     <row r="2" spans="1:37" ht="19.5" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="166" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="O2" s="138"/>
-      <c r="P2" s="138"/>
-      <c r="Q2" s="204"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
+      <c r="P2" s="167"/>
+      <c r="Q2" s="217"/>
       <c r="R2" s="59"/>
       <c r="S2" s="60"/>
       <c r="T2" s="1"/>
@@ -28829,22 +28821,22 @@
     </row>
     <row r="3" spans="1:37" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="139"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="140"/>
-      <c r="O3" s="140"/>
-      <c r="P3" s="140"/>
-      <c r="Q3" s="205"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
+      <c r="L3" s="169"/>
+      <c r="M3" s="169"/>
+      <c r="N3" s="169"/>
+      <c r="O3" s="169"/>
+      <c r="P3" s="169"/>
+      <c r="Q3" s="218"/>
       <c r="R3" s="61"/>
       <c r="S3" s="62"/>
       <c r="T3" s="1"/>
@@ -29003,12 +28995,12 @@
       <c r="E7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="141" t="s">
+      <c r="F7" s="170" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="141"/>
-      <c r="H7" s="141"/>
-      <c r="I7" s="141"/>
+      <c r="G7" s="170"/>
+      <c r="H7" s="170"/>
+      <c r="I7" s="170"/>
       <c r="J7" s="42" t="s">
         <v>76</v>
       </c>
@@ -29061,27 +29053,27 @@
       <c r="AK7" s="1"/>
     </row>
     <row r="8" spans="1:37" ht="33.75" customHeight="1">
-      <c r="A8" s="142" t="s">
+      <c r="A8" s="171" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="220" t="s">
+      <c r="B8" s="212" t="s">
         <v>153</v>
       </c>
-      <c r="C8" s="144" t="s">
+      <c r="C8" s="145" t="s">
         <v>155</v>
       </c>
-      <c r="D8" s="211"/>
-      <c r="E8" s="196" t="s">
+      <c r="D8" s="224"/>
+      <c r="E8" s="183" t="s">
         <v>41</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="16"/>
-      <c r="J8" s="164" t="s">
+      <c r="J8" s="154" t="s">
         <v>156</v>
       </c>
-      <c r="K8" s="169">
+      <c r="K8" s="159">
         <v>1</v>
       </c>
       <c r="L8" s="57">
@@ -29128,17 +29120,17 @@
       <c r="AK8" s="1"/>
     </row>
     <row r="9" spans="1:37" ht="33.75" customHeight="1">
-      <c r="A9" s="142"/>
-      <c r="B9" s="220"/>
-      <c r="C9" s="145"/>
-      <c r="D9" s="162"/>
+      <c r="A9" s="171"/>
+      <c r="B9" s="212"/>
+      <c r="C9" s="146"/>
+      <c r="D9" s="152"/>
       <c r="E9" s="184"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="95"/>
       <c r="I9" s="16"/>
-      <c r="J9" s="180"/>
-      <c r="K9" s="165"/>
+      <c r="J9" s="178"/>
+      <c r="K9" s="155"/>
       <c r="L9" s="57">
         <v>2</v>
       </c>
@@ -29177,17 +29169,17 @@
       <c r="AK9" s="1"/>
     </row>
     <row r="10" spans="1:37" ht="33.75" customHeight="1">
-      <c r="A10" s="142"/>
-      <c r="B10" s="220"/>
-      <c r="C10" s="146"/>
-      <c r="D10" s="163"/>
+      <c r="A10" s="171"/>
+      <c r="B10" s="212"/>
+      <c r="C10" s="147"/>
+      <c r="D10" s="153"/>
       <c r="E10" s="185"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="95"/>
       <c r="I10" s="16"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="166"/>
+      <c r="J10" s="179"/>
+      <c r="K10" s="156"/>
       <c r="L10" s="57">
         <v>3</v>
       </c>
@@ -29226,23 +29218,23 @@
       <c r="AK10" s="1"/>
     </row>
     <row r="11" spans="1:37" ht="33.75" customHeight="1">
-      <c r="A11" s="142"/>
-      <c r="B11" s="220"/>
-      <c r="C11" s="216" t="s">
+      <c r="A11" s="171"/>
+      <c r="B11" s="212"/>
+      <c r="C11" s="209" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="161"/>
-      <c r="E11" s="183" t="s">
+      <c r="D11" s="151"/>
+      <c r="E11" s="199" t="s">
         <v>41</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="95"/>
       <c r="I11" s="16"/>
-      <c r="J11" s="164" t="s">
+      <c r="J11" s="154" t="s">
         <v>157</v>
       </c>
-      <c r="K11" s="169">
+      <c r="K11" s="159">
         <v>4</v>
       </c>
       <c r="L11" s="57">
@@ -29283,17 +29275,17 @@
       <c r="AK11" s="1"/>
     </row>
     <row r="12" spans="1:37" ht="33.75" customHeight="1">
-      <c r="A12" s="142"/>
-      <c r="B12" s="220"/>
-      <c r="C12" s="217"/>
-      <c r="D12" s="162"/>
+      <c r="A12" s="171"/>
+      <c r="B12" s="212"/>
+      <c r="C12" s="210"/>
+      <c r="D12" s="152"/>
       <c r="E12" s="184"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="95"/>
       <c r="I12" s="16"/>
-      <c r="J12" s="180"/>
-      <c r="K12" s="165"/>
+      <c r="J12" s="178"/>
+      <c r="K12" s="155"/>
       <c r="L12" s="57">
         <v>2</v>
       </c>
@@ -29332,17 +29324,17 @@
       <c r="AK12" s="1"/>
     </row>
     <row r="13" spans="1:37" ht="36" customHeight="1">
-      <c r="A13" s="142"/>
-      <c r="B13" s="220"/>
-      <c r="C13" s="218"/>
-      <c r="D13" s="167"/>
-      <c r="E13" s="189"/>
+      <c r="A13" s="171"/>
+      <c r="B13" s="212"/>
+      <c r="C13" s="211"/>
+      <c r="D13" s="157"/>
+      <c r="E13" s="200"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="19"/>
       <c r="I13" s="16"/>
-      <c r="J13" s="181"/>
-      <c r="K13" s="166"/>
+      <c r="J13" s="179"/>
+      <c r="K13" s="156"/>
       <c r="L13" s="57">
         <v>3</v>
       </c>
@@ -29387,23 +29379,23 @@
       <c r="AK13" s="1"/>
     </row>
     <row r="14" spans="1:37" ht="36" customHeight="1">
-      <c r="A14" s="142"/>
-      <c r="B14" s="220"/>
-      <c r="C14" s="216" t="s">
+      <c r="A14" s="171"/>
+      <c r="B14" s="212"/>
+      <c r="C14" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="215"/>
-      <c r="E14" s="212" t="s">
+      <c r="D14" s="213"/>
+      <c r="E14" s="225" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="95"/>
       <c r="G14" s="95"/>
       <c r="H14" s="19"/>
       <c r="I14" s="95"/>
-      <c r="J14" s="164" t="s">
+      <c r="J14" s="154" t="s">
         <v>156</v>
       </c>
-      <c r="K14" s="169">
+      <c r="K14" s="159">
         <v>2</v>
       </c>
       <c r="L14" s="57">
@@ -29444,17 +29436,17 @@
       <c r="AK14" s="1"/>
     </row>
     <row r="15" spans="1:37" ht="36" customHeight="1">
-      <c r="A15" s="142"/>
-      <c r="B15" s="220"/>
-      <c r="C15" s="217"/>
-      <c r="D15" s="215"/>
-      <c r="E15" s="213"/>
+      <c r="A15" s="171"/>
+      <c r="B15" s="212"/>
+      <c r="C15" s="210"/>
+      <c r="D15" s="213"/>
+      <c r="E15" s="215"/>
       <c r="F15" s="95"/>
       <c r="G15" s="95"/>
       <c r="H15" s="19"/>
       <c r="I15" s="95"/>
-      <c r="J15" s="180"/>
-      <c r="K15" s="165"/>
+      <c r="J15" s="178"/>
+      <c r="K15" s="155"/>
       <c r="L15" s="57">
         <v>2</v>
       </c>
@@ -29464,7 +29456,7 @@
       <c r="N15" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="O15" s="209">
+      <c r="O15" s="222">
         <v>2</v>
       </c>
       <c r="P15" s="71">
@@ -29493,17 +29485,17 @@
       <c r="AK15" s="1"/>
     </row>
     <row r="16" spans="1:37" ht="39.75" customHeight="1">
-      <c r="A16" s="142"/>
-      <c r="B16" s="220"/>
-      <c r="C16" s="218"/>
-      <c r="D16" s="215"/>
-      <c r="E16" s="214"/>
+      <c r="A16" s="171"/>
+      <c r="B16" s="212"/>
+      <c r="C16" s="211"/>
+      <c r="D16" s="213"/>
+      <c r="E16" s="216"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="45"/>
-      <c r="J16" s="181"/>
-      <c r="K16" s="166"/>
+      <c r="J16" s="179"/>
+      <c r="K16" s="156"/>
       <c r="L16" s="57">
         <v>3</v>
       </c>
@@ -29513,7 +29505,7 @@
       <c r="N16" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="O16" s="210"/>
+      <c r="O16" s="223"/>
       <c r="P16" s="71">
         <v>0</v>
       </c>
@@ -29546,23 +29538,23 @@
       <c r="AK16" s="1"/>
     </row>
     <row r="17" spans="1:37" ht="39.75" customHeight="1">
-      <c r="A17" s="142"/>
-      <c r="B17" s="220"/>
-      <c r="C17" s="216" t="s">
+      <c r="A17" s="171"/>
+      <c r="B17" s="212"/>
+      <c r="C17" s="209" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="151"/>
-      <c r="E17" s="151" t="s">
+      <c r="D17" s="163"/>
+      <c r="E17" s="163" t="s">
         <v>160</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="45"/>
-      <c r="J17" s="164" t="s">
+      <c r="J17" s="154" t="s">
         <v>156</v>
       </c>
-      <c r="K17" s="169">
+      <c r="K17" s="159">
         <v>3</v>
       </c>
       <c r="L17" s="57">
@@ -29603,17 +29595,17 @@
       <c r="AK17" s="1"/>
     </row>
     <row r="18" spans="1:37" ht="39.75" customHeight="1">
-      <c r="A18" s="142"/>
-      <c r="B18" s="220"/>
-      <c r="C18" s="217"/>
-      <c r="D18" s="152"/>
-      <c r="E18" s="152"/>
+      <c r="A18" s="171"/>
+      <c r="B18" s="212"/>
+      <c r="C18" s="210"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="45"/>
-      <c r="J18" s="180"/>
-      <c r="K18" s="165"/>
+      <c r="J18" s="178"/>
+      <c r="K18" s="155"/>
       <c r="L18" s="57">
         <v>2</v>
       </c>
@@ -29623,7 +29615,7 @@
       <c r="N18" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="O18" s="209">
+      <c r="O18" s="222">
         <v>2</v>
       </c>
       <c r="P18" s="71">
@@ -29652,17 +29644,17 @@
       <c r="AK18" s="1"/>
     </row>
     <row r="19" spans="1:37" ht="39.75" customHeight="1">
-      <c r="A19" s="142"/>
-      <c r="B19" s="220"/>
-      <c r="C19" s="218"/>
-      <c r="D19" s="154"/>
-      <c r="E19" s="154"/>
+      <c r="A19" s="171"/>
+      <c r="B19" s="212"/>
+      <c r="C19" s="211"/>
+      <c r="D19" s="165"/>
+      <c r="E19" s="165"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="19"/>
       <c r="I19" s="45"/>
-      <c r="J19" s="181"/>
-      <c r="K19" s="166"/>
+      <c r="J19" s="179"/>
+      <c r="K19" s="156"/>
       <c r="L19" s="57">
         <v>3</v>
       </c>
@@ -29672,7 +29664,7 @@
       <c r="N19" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="O19" s="210"/>
+      <c r="O19" s="223"/>
       <c r="P19" s="71">
         <v>0</v>
       </c>
@@ -29699,27 +29691,27 @@
       <c r="AK19" s="1"/>
     </row>
     <row r="20" spans="1:37" ht="29.25" customHeight="1">
-      <c r="A20" s="142"/>
-      <c r="B20" s="220"/>
+      <c r="A20" s="171"/>
+      <c r="B20" s="212"/>
       <c r="C20" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="206" t="s">
+      <c r="D20" s="219" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="207"/>
-      <c r="F20" s="207"/>
-      <c r="G20" s="207"/>
-      <c r="H20" s="207"/>
-      <c r="I20" s="207"/>
-      <c r="J20" s="207"/>
-      <c r="K20" s="207"/>
-      <c r="L20" s="207"/>
-      <c r="M20" s="207"/>
-      <c r="N20" s="207"/>
-      <c r="O20" s="207"/>
-      <c r="P20" s="207"/>
-      <c r="Q20" s="208"/>
+      <c r="E20" s="220"/>
+      <c r="F20" s="220"/>
+      <c r="G20" s="220"/>
+      <c r="H20" s="220"/>
+      <c r="I20" s="220"/>
+      <c r="J20" s="220"/>
+      <c r="K20" s="220"/>
+      <c r="L20" s="220"/>
+      <c r="M20" s="220"/>
+      <c r="N20" s="220"/>
+      <c r="O20" s="220"/>
+      <c r="P20" s="220"/>
+      <c r="Q20" s="221"/>
       <c r="R20" s="7"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
@@ -29742,27 +29734,27 @@
       <c r="AK20" s="1"/>
     </row>
     <row r="21" spans="1:37" ht="29.25" customHeight="1">
-      <c r="A21" s="143" t="s">
+      <c r="A21" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="216" t="s">
+      <c r="B21" s="209" t="s">
         <v>154</v>
       </c>
-      <c r="C21" s="216" t="s">
+      <c r="C21" s="209" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="215"/>
-      <c r="E21" s="219" t="s">
+      <c r="D21" s="213"/>
+      <c r="E21" s="214" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="95"/>
       <c r="G21" s="95"/>
       <c r="H21" s="20"/>
       <c r="I21" s="95"/>
-      <c r="J21" s="164" t="s">
+      <c r="J21" s="154" t="s">
         <v>158</v>
       </c>
-      <c r="K21" s="169">
+      <c r="K21" s="159">
         <v>5</v>
       </c>
       <c r="L21" s="57">
@@ -29803,17 +29795,17 @@
       <c r="AK21" s="1"/>
     </row>
     <row r="22" spans="1:37" ht="29.25" customHeight="1">
-      <c r="A22" s="150"/>
-      <c r="B22" s="217"/>
-      <c r="C22" s="217"/>
-      <c r="D22" s="215"/>
-      <c r="E22" s="213"/>
+      <c r="A22" s="161"/>
+      <c r="B22" s="210"/>
+      <c r="C22" s="210"/>
+      <c r="D22" s="213"/>
+      <c r="E22" s="215"/>
       <c r="F22" s="95"/>
       <c r="G22" s="95"/>
       <c r="H22" s="20"/>
       <c r="I22" s="95"/>
-      <c r="J22" s="180"/>
-      <c r="K22" s="165"/>
+      <c r="J22" s="178"/>
+      <c r="K22" s="155"/>
       <c r="L22" s="57">
         <v>2</v>
       </c>
@@ -29852,17 +29844,17 @@
       <c r="AK22" s="1"/>
     </row>
     <row r="23" spans="1:37" ht="29.25" customHeight="1">
-      <c r="A23" s="150"/>
-      <c r="B23" s="217"/>
-      <c r="C23" s="217"/>
-      <c r="D23" s="215"/>
-      <c r="E23" s="213"/>
+      <c r="A23" s="161"/>
+      <c r="B23" s="210"/>
+      <c r="C23" s="210"/>
+      <c r="D23" s="213"/>
+      <c r="E23" s="215"/>
       <c r="F23" s="95"/>
       <c r="G23" s="95"/>
       <c r="H23" s="20"/>
       <c r="I23" s="95"/>
-      <c r="J23" s="180"/>
-      <c r="K23" s="165"/>
+      <c r="J23" s="178"/>
+      <c r="K23" s="155"/>
       <c r="L23" s="57">
         <v>3</v>
       </c>
@@ -29901,17 +29893,17 @@
       <c r="AK23" s="1"/>
     </row>
     <row r="24" spans="1:37" ht="45.75" customHeight="1">
-      <c r="A24" s="153"/>
-      <c r="B24" s="218"/>
-      <c r="C24" s="218"/>
-      <c r="D24" s="215"/>
-      <c r="E24" s="214"/>
+      <c r="A24" s="162"/>
+      <c r="B24" s="211"/>
+      <c r="C24" s="211"/>
+      <c r="D24" s="213"/>
+      <c r="E24" s="216"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="47"/>
-      <c r="J24" s="181"/>
-      <c r="K24" s="166"/>
+      <c r="J24" s="179"/>
+      <c r="K24" s="156"/>
       <c r="L24" s="57">
         <v>4</v>
       </c>
@@ -38434,24 +38426,6 @@
     <filterColumn colId="8" hiddenButton="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="34">
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="A8:A20"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B8:B20"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="K21:K24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="J21:J24"/>
     <mergeCell ref="B2:Q3"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="D20:Q20"/>
@@ -38468,6 +38442,24 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="E11:E13"/>
+    <mergeCell ref="K21:K24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="J21:J24"/>
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A8:A20"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B8:B20"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -38544,24 +38536,24 @@
     </row>
     <row r="2" spans="1:37" ht="19.5" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="166" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="O2" s="138"/>
-      <c r="P2" s="138"/>
-      <c r="Q2" s="138"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="167"/>
+      <c r="I2" s="167"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="167"/>
+      <c r="L2" s="167"/>
+      <c r="M2" s="167"/>
+      <c r="N2" s="167"/>
+      <c r="O2" s="167"/>
+      <c r="P2" s="167"/>
+      <c r="Q2" s="167"/>
       <c r="R2" s="59"/>
       <c r="S2" s="60"/>
       <c r="T2" s="1"/>
@@ -38585,22 +38577,22 @@
     </row>
     <row r="3" spans="1:37" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="139"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="140"/>
-      <c r="O3" s="140"/>
-      <c r="P3" s="140"/>
-      <c r="Q3" s="140"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
+      <c r="L3" s="169"/>
+      <c r="M3" s="169"/>
+      <c r="N3" s="169"/>
+      <c r="O3" s="169"/>
+      <c r="P3" s="169"/>
+      <c r="Q3" s="169"/>
       <c r="R3" s="61"/>
       <c r="S3" s="62"/>
       <c r="T3" s="1"/>
@@ -38759,12 +38751,12 @@
       <c r="E7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="141" t="s">
+      <c r="F7" s="170" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="141"/>
-      <c r="H7" s="141"/>
-      <c r="I7" s="141"/>
+      <c r="G7" s="170"/>
+      <c r="H7" s="170"/>
+      <c r="I7" s="170"/>
       <c r="J7" s="42" t="s">
         <v>76</v>
       </c>
@@ -38817,25 +38809,25 @@
       <c r="AK7" s="1"/>
     </row>
     <row r="8" spans="1:37" ht="33" customHeight="1">
-      <c r="A8" s="142" t="s">
+      <c r="A8" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="222" t="s">
+      <c r="B8" s="227" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="223"/>
-      <c r="D8" s="193"/>
-      <c r="E8" s="228" t="s">
+      <c r="C8" s="228"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="233" t="s">
         <v>43</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="15"/>
-      <c r="J8" s="164" t="s">
+      <c r="J8" s="154" t="s">
         <v>77</v>
       </c>
-      <c r="K8" s="164">
+      <c r="K8" s="154">
         <v>1</v>
       </c>
       <c r="L8" s="57">
@@ -38880,17 +38872,17 @@
       <c r="AK8" s="1"/>
     </row>
     <row r="9" spans="1:37" ht="33" customHeight="1">
-      <c r="A9" s="142"/>
-      <c r="B9" s="224"/>
-      <c r="C9" s="225"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="229"/>
+      <c r="A9" s="171"/>
+      <c r="B9" s="229"/>
+      <c r="C9" s="230"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="234"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="15"/>
-      <c r="J9" s="165"/>
-      <c r="K9" s="180"/>
+      <c r="J9" s="155"/>
+      <c r="K9" s="178"/>
       <c r="L9" s="57">
         <v>2</v>
       </c>
@@ -38929,17 +38921,17 @@
       <c r="AK9" s="1"/>
     </row>
     <row r="10" spans="1:37" ht="33" customHeight="1">
-      <c r="A10" s="142"/>
-      <c r="B10" s="224"/>
-      <c r="C10" s="225"/>
-      <c r="D10" s="194"/>
-      <c r="E10" s="229"/>
+      <c r="A10" s="171"/>
+      <c r="B10" s="229"/>
+      <c r="C10" s="230"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="234"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="15"/>
-      <c r="J10" s="165"/>
-      <c r="K10" s="180"/>
+      <c r="J10" s="155"/>
+      <c r="K10" s="178"/>
       <c r="L10" s="57">
         <v>3</v>
       </c>
@@ -38978,17 +38970,17 @@
       <c r="AK10" s="1"/>
     </row>
     <row r="11" spans="1:37" ht="33" customHeight="1">
-      <c r="A11" s="142"/>
-      <c r="B11" s="224"/>
-      <c r="C11" s="225"/>
-      <c r="D11" s="194"/>
-      <c r="E11" s="229"/>
+      <c r="A11" s="171"/>
+      <c r="B11" s="229"/>
+      <c r="C11" s="230"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="234"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="15"/>
-      <c r="J11" s="165"/>
-      <c r="K11" s="180"/>
+      <c r="J11" s="155"/>
+      <c r="K11" s="178"/>
       <c r="L11" s="57">
         <v>4</v>
       </c>
@@ -39025,17 +39017,17 @@
       <c r="AK11" s="1"/>
     </row>
     <row r="12" spans="1:37" ht="33" customHeight="1">
-      <c r="A12" s="142"/>
-      <c r="B12" s="226"/>
-      <c r="C12" s="227"/>
-      <c r="D12" s="195"/>
-      <c r="E12" s="230"/>
+      <c r="A12" s="171"/>
+      <c r="B12" s="231"/>
+      <c r="C12" s="232"/>
+      <c r="D12" s="182"/>
+      <c r="E12" s="235"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="15"/>
-      <c r="J12" s="166"/>
-      <c r="K12" s="181"/>
+      <c r="J12" s="156"/>
+      <c r="K12" s="179"/>
       <c r="L12" s="57">
         <v>5</v>
       </c>
@@ -39072,7 +39064,7 @@
       <c r="AK12" s="1"/>
     </row>
     <row r="13" spans="1:37" ht="33" customHeight="1">
-      <c r="A13" s="142"/>
+      <c r="A13" s="171"/>
       <c r="B13" s="43" t="s">
         <v>15</v>
       </c>
@@ -39137,8 +39129,8 @@
       <c r="AK13" s="1"/>
     </row>
     <row r="14" spans="1:37" ht="33" customHeight="1">
-      <c r="A14" s="142"/>
-      <c r="B14" s="186" t="s">
+      <c r="A14" s="171"/>
+      <c r="B14" s="196" t="s">
         <v>181</v>
       </c>
       <c r="C14" s="44" t="s">
@@ -39200,8 +39192,8 @@
       <c r="AK14" s="1"/>
     </row>
     <row r="15" spans="1:37" ht="33" customHeight="1">
-      <c r="A15" s="142"/>
-      <c r="B15" s="187"/>
+      <c r="A15" s="171"/>
+      <c r="B15" s="197"/>
       <c r="C15" s="44" t="s">
         <v>85</v>
       </c>
@@ -39255,7 +39247,7 @@
       <c r="AK15" s="1"/>
     </row>
     <row r="16" spans="1:37" ht="33" customHeight="1">
-      <c r="A16" s="142"/>
+      <c r="A16" s="171"/>
       <c r="B16" s="43" t="s">
         <v>35</v>
       </c>
@@ -39314,7 +39306,7 @@
       <c r="AK16" s="1"/>
     </row>
     <row r="17" spans="1:37" ht="33" customHeight="1">
-      <c r="A17" s="142"/>
+      <c r="A17" s="171"/>
       <c r="B17" s="44" t="s">
         <v>37</v>
       </c>
@@ -39373,8 +39365,8 @@
       <c r="AK17" s="1"/>
     </row>
     <row r="18" spans="1:37" ht="33" customHeight="1">
-      <c r="A18" s="142"/>
-      <c r="B18" s="221" t="s">
+      <c r="A18" s="171"/>
+      <c r="B18" s="226" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="43" t="s">
@@ -39428,8 +39420,8 @@
       <c r="AK18" s="1"/>
     </row>
     <row r="19" spans="1:37" ht="33" customHeight="1">
-      <c r="A19" s="142"/>
-      <c r="B19" s="221"/>
+      <c r="A19" s="171"/>
+      <c r="B19" s="226"/>
       <c r="C19" s="43" t="s">
         <v>93</v>
       </c>

</xml_diff>